<commit_message>
update 3d printed parts board
</commit_message>
<xml_diff>
--- a/printed_parts/3D printed parts excel board.xlsx
+++ b/printed_parts/3D printed parts excel board.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$H$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>NAME</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Qte / machine</t>
+  </si>
+  <si>
+    <t>DOORLOCKER</t>
   </si>
 </sst>
 </file>
@@ -503,13 +506,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>866880</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>867620</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>1294560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1017,13 +1020,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>866880</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>867620</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>1294560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1054,13 +1057,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>650876</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1967595</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>1377950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1834,6 +1837,50 @@
         <a:xfrm>
           <a:off x="4200525" y="6810375"/>
           <a:ext cx="1905000" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1076325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2524125</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Image 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4391025" y="39338250"/>
+          <a:ext cx="2009775" cy="2009775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2170,10 +2217,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -2192,8 +2239,8 @@
         <v>23</v>
       </c>
       <c r="C1" s="9">
-        <f>SUM(F4:F60)</f>
-        <v>40</v>
+        <f>SUM(F4:F61)</f>
+        <v>42</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2207,7 +2254,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="9">
-        <f>SUM(H4:H60)</f>
+        <f>SUM(H4:H61)</f>
         <v>0</v>
       </c>
       <c r="D2" s="10">
@@ -2275,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="14">
-        <f t="shared" ref="F5:F31" si="0">E5*C5</f>
+        <f t="shared" ref="F5:F32" si="0">E5*C5</f>
         <v>2</v>
       </c>
       <c r="G5" s="11"/>
@@ -2758,27 +2805,46 @@
       <c r="G30" s="11"/>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="1:11" s="2" customFormat="1" ht="113.1" customHeight="1">
+    <row r="31" spans="1:11" ht="113.1" customHeight="1">
       <c r="A31" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15">
-        <v>1</v>
-      </c>
-      <c r="D31" s="15"/>
+        <v>37</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16">
+        <v>2</v>
+      </c>
+      <c r="D31" s="11"/>
       <c r="E31" s="13">
         <v>1</v>
       </c>
       <c r="F31" s="14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="11"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" s="2" customFormat="1" ht="113.1" customHeight="1">
+      <c r="A32" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15">
+        <v>1</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="13">
+        <v>1</v>
+      </c>
+      <c r="F32" s="14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>